<commit_message>
Integrate xlsx-mode into CLI option
</commit_message>
<xml_diff>
--- a/test/data2/in.xlsx
+++ b/test/data2/in.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -566,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Support direct range notation
</commit_message>
<xml_diff>
--- a/test/data2/in.xlsx
+++ b/test/data2/in.xlsx
@@ -11,8 +11,8 @@
     <sheet name="charts" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="chart_sidebyside">charts!$A$1:$A$4,charts!$D$1:$D$4</definedName>
-    <definedName name="chart01">charts!$A$1:$D$4</definedName>
+    <definedName name="chart_sidebyside">charts!$A$1:$A$5,charts!$D$1:$D$5</definedName>
+    <definedName name="chart01">charts!$A$1:$D$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Slide ID</t>
     <phoneticPr fontId="1"/>
@@ -128,6 +128,17 @@
   </si>
   <si>
     <t>SideBySide</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>冬</t>
+    <rPh sb="0" eb="1">
+      <t>フユ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>normal2</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -453,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -504,27 +515,25 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
+        <v>29</v>
+      </c>
+      <c r="D4" t="e">
+        <f>charts!A7:D9,charts!A10:D11</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -532,26 +541,40 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -564,10 +587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D4"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -628,6 +651,90 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>130</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>110</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>120</v>
+      </c>
+      <c r="C10">
+        <v>70</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>130</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>